<commit_message>
resolved merge function, tidied notebook
</commit_message>
<xml_diff>
--- a/SEFL/SEFL_Inactivity_Cohort_1.xlsx
+++ b/SEFL/SEFL_Inactivity_Cohort_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brelw\IntroPython\IntroPythonGit\IntroPythonCourse_2022\SEFL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3743926E-4DFC-4DA6-AF00-4CD16E23BB54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9843691D-507C-4AC3-A0EE-0643E32B5052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11048" yWindow="503" windowWidth="15127" windowHeight="12360" xr2:uid="{127E7744-B7EA-4C52-88B0-51FF8FF6D69F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" xr2:uid="{127E7744-B7EA-4C52-88B0-51FF8FF6D69F}"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2373" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2370" uniqueCount="68">
   <si>
     <t/>
   </si>
@@ -600,7 +600,7 @@
   <dimension ref="A1:O387"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="C299" sqref="C299"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -621,40 +621,40 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.45">
@@ -668,40 +668,40 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.45">
@@ -715,40 +715,40 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.45">
@@ -762,87 +762,78 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="K4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="L4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="O4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>0</v>
-      </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="J5" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="K5" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="L5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="M5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="N5" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="O5" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.45">

</xml_diff>